<commit_message>
Cambios en truncamiento de códigos de recursos
Cambios en truncamiento de códigos de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion10/ESCALETA FINAL CN_11_10_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion10/ESCALETA FINAL CN_11_10_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado11\guion10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$49</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1517,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,7 +1933,7 @@
         <v>145</v>
       </c>
       <c r="H9" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>19</v>
@@ -1992,7 +1992,7 @@
         <v>143</v>
       </c>
       <c r="H10" s="66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10" s="66" t="s">
         <v>20</v>
@@ -5129,11 +5129,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -5149,6 +5144,11 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>